<commit_message>
add list2 to dz
</commit_message>
<xml_diff>
--- a/dz.xlsx
+++ b/dz.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Frontend\git\archpc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\29504867\Documents\GIT\archpc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>X</t>
   </si>
@@ -45,13 +46,88 @@
   </si>
   <si>
     <t>(X-&gt;Y)or Z</t>
+  </si>
+  <si>
+    <t>(Y or Z &lt;=&gt; X) or ((X-&gt;Y)or Z)</t>
+  </si>
+  <si>
+    <t>a0=1</t>
+  </si>
+  <si>
+    <t>a0=0</t>
+  </si>
+  <si>
+    <t>a1=1</t>
+  </si>
+  <si>
+    <t>a3+a0=1</t>
+  </si>
+  <si>
+    <t>a2+a0=1</t>
+  </si>
+  <si>
+    <t>a2+a3+a23+a0=1</t>
+  </si>
+  <si>
+    <t>a1+a0=0</t>
+  </si>
+  <si>
+    <t>a1+a3+a13+a0=1</t>
+  </si>
+  <si>
+    <t>a1+a2+a12+a0=1</t>
+  </si>
+  <si>
+    <t>a123+a12+a13+a23+a1+a2+a3+a0=0</t>
+  </si>
+  <si>
+    <t>построение Полинома Жегалкина</t>
+  </si>
+  <si>
+    <t>1=1</t>
+  </si>
+  <si>
+    <t>0+1=1</t>
+  </si>
+  <si>
+    <t>0+1</t>
+  </si>
+  <si>
+    <t>0+0+0+1=1</t>
+  </si>
+  <si>
+    <t>1+1=0</t>
+  </si>
+  <si>
+    <t>1+0+1+1=1</t>
+  </si>
+  <si>
+    <t>1+1+1+0+1+0+0+1=1</t>
+  </si>
+  <si>
+    <t>a3=0</t>
+  </si>
+  <si>
+    <t>a2=0</t>
+  </si>
+  <si>
+    <t>a23=0</t>
+  </si>
+  <si>
+    <t>a13=1</t>
+  </si>
+  <si>
+    <t>a12=1</t>
+  </si>
+  <si>
+    <t>a123=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +135,20 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,9 +171,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -366,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,4 +707,339 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>OR(B2,C2)*1</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>OR(NOT(A2),B2)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>OR(F2,C2)*1</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" si="0">OR(B3,C3)*1</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="1">OR(NOT(A3),B3)*1</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="2">OR(F3,C3)*1</f>
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add list3 to dz
</commit_message>
<xml_diff>
--- a/dz.xlsx
+++ b/dz.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>X</t>
   </si>
@@ -121,6 +122,9 @@
   </si>
   <si>
     <t>a123=1</t>
+  </si>
+  <si>
+    <t>F=nXnYnZ+nXnYZ+nXYnZ+nXYZ+XnYZ+XYnZ</t>
   </si>
 </sst>
 </file>
@@ -171,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -179,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,4 +1049,298 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>IF(OR(B2=1,C2=1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>IF(D2=A2,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>IF(A2=1,B2,1)</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>IF(OR(F2=1,C2=1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <f>IF(OR(E2=1,G2=1),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" si="0">IF(OR(B3=1,C3=1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">IF(D3=A3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="2">IF(A3=1,B3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="3">IF(OR(F3=1,C3=1),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H8" si="4">IF(OR(E3=1,G3=1),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <f>IF(OR(E9=1,G9=1),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upd list3 to dz
</commit_message>
<xml_diff>
--- a/dz.xlsx
+++ b/dz.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>X</t>
   </si>
@@ -721,7 +721,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H8" si="4">IF(OR(E3=1,G3=1),1,0)</f>
+        <f t="shared" ref="H3:H9" si="4">IF(OR(E3=1,G3=1),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1336,8 +1336,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <f>IF(OR(E9=1,G9=1),1,0)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
triangle pascal add and complete
</commit_message>
<xml_diff>
--- a/dz.xlsx
+++ b/dz.xlsx
@@ -145,9 +145,6 @@
     <t>XnYZ</t>
   </si>
   <si>
-    <t>Xynz</t>
-  </si>
-  <si>
     <t>XYZ</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>F СДНФ</t>
+  </si>
+  <si>
+    <t>XYnZ</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,10 +1125,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1400,17 +1400,17 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>